<commit_message>
update file, mass flow rate of fuel
</commit_message>
<xml_diff>
--- a/cgam-berechnungen-aus-tdo.xlsx
+++ b/cgam-berechnungen-aus-tdo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CGAM" sheetId="4" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="147">
   <si>
     <t>CGAM Berechnungen, nach TDO</t>
   </si>
@@ -909,6 +909,15 @@
   </si>
   <si>
     <t>h5</t>
+  </si>
+  <si>
+    <t>Massenstrom Brennstoff</t>
+  </si>
+  <si>
+    <t>m_fuel</t>
+  </si>
+  <si>
+    <t>LHV (kJ/kg)</t>
   </si>
 </sst>
 </file>
@@ -2805,22 +2814,22 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>51</v>
       </c>
@@ -2840,7 +2849,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20" t="s">
@@ -2856,7 +2865,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="20">
         <v>1</v>
       </c>
@@ -2877,7 +2886,7 @@
         <v>1.0129999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="20">
         <v>2</v>
       </c>
@@ -2898,7 +2907,7 @@
         <v>10.130000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>3</v>
       </c>
@@ -2919,7 +2928,7 @@
         <v>9.6229999999999993</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="20">
         <v>4</v>
       </c>
@@ -2940,7 +2949,7 @@
         <v>9.1419999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="20">
         <v>5</v>
       </c>
@@ -2961,7 +2970,7 @@
         <v>1.099</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="20">
         <v>6</v>
       </c>
@@ -2982,7 +2991,7 @@
         <v>1.0660000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="20">
         <v>7</v>
       </c>
@@ -3003,7 +3012,7 @@
         <v>1.0129999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
         <v>8</v>
       </c>
@@ -3024,7 +3033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="20">
         <v>9</v>
       </c>
@@ -3045,7 +3054,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="20">
         <v>10</v>
       </c>
@@ -3066,7 +3075,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>62</v>
       </c>
@@ -3075,7 +3084,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
         <v>58</v>
       </c>
@@ -3087,7 +3096,7 @@
         <v>28.648826980000003</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>59</v>
       </c>
@@ -3099,7 +3108,7 @@
         <v>28.2556291</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
         <v>61</v>
       </c>
@@ -3111,7 +3120,7 @@
         <v>16.0426</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
         <v>63</v>
       </c>
@@ -3134,7 +3143,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
         <v>58</v>
       </c>
@@ -3158,7 +3167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
         <v>59</v>
       </c>
@@ -3182,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
         <v>61</v>
       </c>
@@ -3220,18 +3229,18 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -3257,7 +3266,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3290,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3323,7 +3332,7 @@
         <v>27.5382</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3356,7 +3365,7 @@
         <v>41.938400000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3389,7 +3398,7 @@
         <v>101.4538</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3422,7 +3431,7 @@
         <v>38.782299999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3455,7 +3464,7 @@
         <v>21.7516</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3488,7 +3497,7 @@
         <v>2.7726000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3521,7 +3530,7 @@
         <v>6.1600000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3554,7 +3563,7 @@
         <v>12.8102</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3587,7 +3596,7 @@
         <v>84.993899999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" s="26"/>
     </row>
   </sheetData>
@@ -3599,18 +3608,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -3618,7 +3627,7 @@
         <v>-4713.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -3630,12 +3639,12 @@
         <v>29662.292650354288</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -3643,7 +3652,7 @@
         <v>9304.9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -3666,28 +3675,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>73</v>
       </c>
@@ -3701,7 +3710,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="20"/>
       <c r="B5" s="20">
         <f>850/10^3</f>
@@ -3713,7 +3722,7 @@
       </c>
       <c r="D5" s="23"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>64</v>
       </c>
@@ -3733,7 +3742,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>64</v>
       </c>
@@ -3750,7 +3759,7 @@
         <v>22276.447747368431</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>65</v>
       </c>
@@ -3767,7 +3776,7 @@
         <v>23597.861656343652</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>66</v>
       </c>
@@ -3784,7 +3793,7 @@
         <v>36961.945674303395</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>76</v>
       </c>
@@ -3801,12 +3810,12 @@
         <v>29037.924364860693</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="20"/>
       <c r="B13" s="20" t="s">
         <v>81</v>
@@ -3816,7 +3825,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
         <v>61</v>
       </c>
@@ -3833,7 +3842,7 @@
         <v>-74871.971532006879</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
         <v>65</v>
       </c>
@@ -3853,7 +3862,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
         <v>66</v>
       </c>
@@ -3870,7 +3879,7 @@
         <v>-393520.99342271435</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>76</v>
       </c>
@@ -3887,13 +3896,16 @@
         <v>-241854.53998521887</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="20"/>
       <c r="B19" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>61</v>
       </c>
@@ -3901,13 +3913,17 @@
         <f>D14+D15-D16-2*D17</f>
         <v>802357.40262233443</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="20">
+        <f>B20/CGAM!C21</f>
+        <v>50014.17492316298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="23" t="s">
         <v>84</v>
       </c>
@@ -3916,12 +3932,12 @@
         <v>3.2122888972033976E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
         <v>63</v>
       </c>
@@ -3938,7 +3954,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
         <v>59</v>
       </c>
@@ -3957,6 +3973,23 @@
       <c r="E27" s="20">
         <f>(CGAM!E24+2*B23)/(1+B23)</f>
         <v>8.0654909249206222E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="20">
+        <f>B23*(CGAM!C21/CGAM!C19)*CGAM!C7</f>
+        <v>1.6418658862678763</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3972,27 +4005,27 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>73</v>
       </c>
@@ -4006,7 +4039,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="20"/>
       <c r="B7" s="20">
         <f>603.738/10^3</f>
@@ -4018,7 +4051,7 @@
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
         <v>64</v>
       </c>
@@ -4038,7 +4071,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>64</v>
       </c>
@@ -4055,7 +4088,7 @@
         <v>7831.9633258017038</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>65</v>
       </c>
@@ -4072,7 +4105,7 @@
         <v>8117.0220833391722</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>66</v>
       </c>
@@ -4089,7 +4122,7 @@
         <v>12667.817108231946</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>76</v>
       </c>
@@ -4106,7 +4139,7 @@
         <v>9666.0552025948127</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>91</v>
       </c>
@@ -4114,7 +4147,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15">
         <f>B9*CGAM!B24+APH!B10*CGAM!C24+APH!B11*CGAM!D24+APH!B12*CGAM!E24</f>
         <v>4596.9248442635608</v>
@@ -4128,7 +4161,7 @@
         <v>-7926.9554257724694</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -4137,7 +4170,7 @@
         <v>3.1859995113267479</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -4146,17 +4179,17 @@
         <v>-25255.27611282</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
         <v>73</v>
       </c>
@@ -4170,7 +4203,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="20"/>
       <c r="B24" s="20">
         <f>1006.162/10^3</f>
@@ -4182,7 +4215,7 @@
       </c>
       <c r="D24" s="23"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
         <v>64</v>
       </c>
@@ -4202,7 +4235,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
         <v>64</v>
       </c>
@@ -4219,7 +4252,7 @@
         <v>-7331.5638839222629</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
         <v>65</v>
       </c>
@@ -4236,7 +4269,7 @@
         <v>-7671.4905703082131</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
         <v>66</v>
       </c>
@@ -4253,7 +4286,7 @@
         <v>-12033.391588182887</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="20" t="s">
         <v>76</v>
       </c>
@@ -4270,7 +4303,7 @@
         <v>-9244.9754267340468</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>99</v>
       </c>
@@ -4278,7 +4311,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32">
         <f>B26*CGAM!B25+APH!B27*CGAM!C25+APH!B28*CGAM!D25+APH!B29*CGAM!E25</f>
         <v>-8844.5937848635804</v>
@@ -4292,7 +4325,7 @@
         <v>7680.2515267131093</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -4301,7 +4334,7 @@
         <v>3.2886529340978266</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -4324,24 +4357,24 @@
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>73</v>
       </c>
@@ -4355,7 +4388,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="20"/>
       <c r="B7" s="20">
         <f>779.784/10^3</f>
@@ -4367,7 +4400,7 @@
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
         <v>64</v>
       </c>
@@ -4387,7 +4420,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>64</v>
       </c>
@@ -4404,7 +4437,7 @@
         <v>-11023.463593086573</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>65</v>
       </c>
@@ -4421,7 +4454,7 @@
         <v>-11337.67178829331</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>66</v>
       </c>
@@ -4438,7 +4471,7 @@
         <v>-17415.14579566929</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>76</v>
       </c>
@@ -4455,7 +4488,7 @@
         <v>-13351.865389281738</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>100</v>
       </c>
@@ -4463,7 +4496,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15">
         <f>B9*CGAM!$B$25+B10*CGAM!$C$25+B11*CGAM!$D$25+B12*CGAM!$E$25</f>
         <v>-16524.84531157669</v>
@@ -4477,7 +4510,7 @@
         <v>11455.173803582984</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -4486,7 +4519,7 @@
         <v>3.2886529340978266</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -4495,10 +4528,10 @@
         <v>37672.09093975374</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B18" s="25"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>113</v>
       </c>
@@ -4506,7 +4539,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -4515,7 +4548,7 @@
         <v>352.887</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -4525,7 +4558,7 @@
       </c>
       <c r="D21" s="25"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
         <v>106</v>
       </c>
@@ -4533,7 +4566,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -4541,7 +4574,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="N26" s="20" t="s">
         <v>73</v>
       </c>
@@ -4555,7 +4588,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>111</v>
       </c>
@@ -4570,7 +4603,7 @@
       </c>
       <c r="Q27" s="23"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>115</v>
       </c>
@@ -4594,7 +4627,7 @@
         <v>-2925.1160801804431</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -4618,7 +4651,7 @@
         <v>-3029.5962641745891</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="N30" s="20" t="s">
         <v>65</v>
       </c>
@@ -4635,7 +4668,7 @@
         <v>-3090.9073909511803</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -4661,7 +4694,7 @@
         <v>-4624.8486955509288</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="N32" s="20" t="s">
         <v>76</v>
       </c>
@@ -4678,7 +4711,7 @@
         <v>-3590.3081301309576</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>112</v>
       </c>
@@ -4689,7 +4722,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>107</v>
       </c>
@@ -4712,7 +4745,7 @@
         <v>3133.34852469623</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>-15866</v>
       </c>
@@ -4731,7 +4764,7 @@
         <v>3.2886529340978266</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>109</v>
       </c>
@@ -4747,7 +4780,7 @@
         <v>10304.495819293354</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -4765,7 +4798,7 @@
         <v>10305.754689333922</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>107</v>
       </c>
@@ -4776,7 +4809,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>106.67698424832</v>
       </c>
@@ -4794,12 +4827,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q43" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="N44" t="s">
         <v>131</v>
       </c>
@@ -4808,7 +4841,7 @@
         <v>1954.8282228900275</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="N45" t="s">
         <v>118</v>
       </c>
@@ -4830,14 +4863,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -4845,7 +4878,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4854,7 +4887,7 @@
         <v>426.89699999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <f>HRSG!O37</f>
         <v>10304.495819293354</v>
@@ -4863,7 +4896,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>HRSG!O37</f>
         <v>10304.495819293354</v>
@@ -4872,7 +4905,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>HRSG!B17</f>
         <v>37672.09093975374</v>
@@ -4882,12 +4915,12 @@
         <v>779.78399999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -4895,7 +4928,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -4904,7 +4937,7 @@
         <v>298.14999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <f>HRSG!O37</f>
         <v>10304.495819293354</v>
@@ -4913,7 +4946,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <f>HRSG!O37</f>
         <v>10304.495819293354</v>
@@ -4923,7 +4956,7 @@
         <v>485.57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <f>HRSG!B17</f>
         <v>37672.09093975374</v>
@@ -4947,23 +4980,23 @@
       <selection activeCell="I7" sqref="I7:P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="15.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="7" width="15.7265625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="11.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -4977,7 +5010,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -4989,7 +5022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I7" s="1" t="s">
         <v>40</v>
       </c>
@@ -5013,7 +5046,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -5049,7 +5082,7 @@
         <v>32.06</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -5060,7 +5093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>8</v>
       </c>
@@ -5068,7 +5101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5094,7 +5127,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -5121,7 +5154,7 @@
         <v>12.010999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
@@ -5148,7 +5181,7 @@
         <v>32.06</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>22</v>
       </c>
@@ -5178,7 +5211,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
@@ -5205,7 +5238,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
@@ -5232,7 +5265,7 @@
         <v>31.998799999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -5259,7 +5292,7 @@
         <v>2.0158</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
@@ -5286,7 +5319,7 @@
         <v>28.010399999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
@@ -5313,7 +5346,7 @@
         <v>44.009799999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
         <v>26</v>
       </c>
@@ -5340,7 +5373,7 @@
         <v>18.0152</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
         <v>27</v>
       </c>
@@ -5367,7 +5400,7 @@
         <v>18.0152</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
         <v>28</v>
       </c>
@@ -5394,7 +5427,7 @@
         <v>16.0426</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
@@ -5424,7 +5457,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A27" s="7" t="s">
         <v>30</v>
       </c>
@@ -5451,7 +5484,7 @@
         <v>64.058800000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" s="7" t="s">
         <v>31</v>
       </c>
@@ -5478,7 +5511,7 @@
         <v>34.075800000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.4">
       <c r="A29" s="7" t="s">
         <v>32</v>
       </c>
@@ -5505,12 +5538,12 @@
         <v>17.0304</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15.5" x14ac:dyDescent="0.4">
       <c r="A35" s="12" t="s">
         <v>9</v>
       </c>
@@ -5527,7 +5560,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>16</v>
       </c>
@@ -5548,7 +5581,7 @@
         <v>-2449.8878542539073</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
@@ -5569,7 +5602,7 @@
         <v>-13190.637189785037</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A38" s="7" t="s">
         <v>22</v>
       </c>
@@ -5590,7 +5623,7 @@
         <v>-77101.864471418376</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" s="7" t="s">
         <v>23</v>
       </c>
@@ -5611,7 +5644,7 @@
         <v>-82521.174962554447</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A40" s="7" t="s">
         <v>24</v>
       </c>
@@ -5632,7 +5665,7 @@
         <v>-52726.949982142716</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -5653,7 +5686,7 @@
         <v>-190047.2101230229</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" s="7" t="s">
         <v>25</v>
       </c>
@@ -5674,7 +5707,7 @@
         <v>-479649.42974581476</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A43" s="7" t="s">
         <v>26</v>
       </c>
@@ -5695,7 +5728,7 @@
         <v>-317904.16410855361</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
         <v>27</v>
       </c>
@@ -5716,7 +5749,7 @@
         <v>-314990.79434255324</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
         <v>28</v>
       </c>
@@ -5737,7 +5770,7 @@
         <v>-149952.50257625582</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A46" s="7" t="s">
         <v>29</v>
       </c>
@@ -5758,7 +5791,7 @@
         <v>-177464.8037282186</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A47" s="7" t="s">
         <v>30</v>
       </c>
@@ -5779,7 +5812,7 @@
         <v>-396707.28944975371</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A48" s="7" t="s">
         <v>31</v>
       </c>
@@ -5800,7 +5833,7 @@
         <v>-103341.4875216347</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A49" s="7" t="s">
         <v>32</v>
       </c>

</xml_diff>